<commit_message>
A bit more... can't remember what's changed.
</commit_message>
<xml_diff>
--- a/video_completion_graphs.xlsx
+++ b/video_completion_graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="12015"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Count</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>97-100%</t>
+  </si>
+  <si>
+    <t>0-20%</t>
+  </si>
+  <si>
+    <t>20-40%</t>
+  </si>
+  <si>
+    <t>40-60%</t>
+  </si>
+  <si>
+    <t>60-80%</t>
+  </si>
+  <si>
+    <t>90-95%</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>95-99%</t>
+  </si>
+  <si>
+    <t>80-90%</t>
   </si>
 </sst>
 </file>
@@ -688,6 +712,377 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="109"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="9"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="0" h="0"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="0" h="0"/>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>0-20%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>20-40%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13570100612423447"/>
+                  <c:y val="3.4231379760164708E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>40-60%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.18644706911636044"/>
+                  <c:y val="3.3269209612271519E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>60-80%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.4063867016622926E-2"/>
+                  <c:y val="9.0150407845725872E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>80-90%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10918438320209974"/>
+                  <c:y val="-4.0079211655429298E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>90-95%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.2242017494971898"/>
+                  <c:y val="-6.5629056846936054E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>95-99%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.3387817389676553E-2"/>
+                  <c:y val="4.8174517107517252E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>100%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$56:$I$63</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0-20%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-40%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40-60%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60-80%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80-90%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90-95%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95-99%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$56:$K$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -777,6 +1172,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1074,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37:K42"/>
+    <sheetView tabSelected="1" topLeftCell="G40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2861,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>109</v>
       </c>
@@ -2457,7 +2884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>109</v>
       </c>
@@ -2480,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>109</v>
       </c>
@@ -2503,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>105</v>
       </c>
@@ -2526,7 +2953,7 @@
         <v>0.94339622641509435</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>109</v>
       </c>
@@ -2549,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>108</v>
       </c>
@@ -2572,7 +2999,7 @@
         <v>0.98113207547169812</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>107</v>
       </c>
@@ -2594,8 +3021,17 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>5</v>
+      </c>
+      <c r="J55" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>109</v>
       </c>
@@ -2617,8 +3053,18 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="K56">
+        <f t="array" ref="K56:K63">FREQUENCY(D2:D241,J56:J63)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>107</v>
       </c>
@@ -2640,8 +3086,17 @@
         <f t="shared" si="2"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J57" s="3">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="K57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>101</v>
       </c>
@@ -2663,8 +3118,17 @@
         <f t="shared" si="2"/>
         <v>0.8867924528301887</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="K58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>109</v>
       </c>
@@ -2686,8 +3150,17 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="K59">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>105</v>
       </c>
@@ -2709,8 +3182,17 @@
         <f t="shared" si="2"/>
         <v>0.92452830188679247</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="K60">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>109</v>
       </c>
@@ -2732,8 +3214,17 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I61" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K61">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>106</v>
       </c>
@@ -2755,8 +3246,17 @@
         <f t="shared" si="2"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="K62">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>109</v>
       </c>
@@ -2778,8 +3278,17 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="3">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>106</v>
       </c>
@@ -2801,8 +3310,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I64" s="2"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>109</v>
       </c>
@@ -2824,8 +3335,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I65" s="2"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>105</v>
       </c>
@@ -2847,8 +3360,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I66" s="2"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>109</v>
       </c>
@@ -2870,8 +3385,10 @@
         <f t="shared" ref="F67:F130" si="5">C67/53</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I67" s="2"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>106</v>
       </c>
@@ -2893,8 +3410,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I68" s="2"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>107</v>
       </c>
@@ -2916,8 +3435,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I69" s="2"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>109</v>
       </c>
@@ -2939,8 +3460,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I70" s="2"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>108</v>
       </c>
@@ -2962,8 +3485,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I71" s="2"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>106</v>
       </c>
@@ -2985,8 +3510,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I72" s="2"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>109</v>
       </c>
@@ -3008,8 +3535,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I73" s="2"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>109</v>
       </c>
@@ -3031,8 +3560,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I74" s="2"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>109</v>
       </c>
@@ -3054,8 +3585,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I75" s="2"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>108</v>
       </c>
@@ -3077,8 +3610,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I76" s="2"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>105</v>
       </c>
@@ -3100,8 +3635,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I77" s="2"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>107</v>
       </c>
@@ -3123,8 +3660,10 @@
         <f t="shared" si="5"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I78" s="2"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>109</v>
       </c>
@@ -3146,8 +3685,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I79" s="2"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>109</v>
       </c>
@@ -3169,8 +3710,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I80" s="2"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>109</v>
       </c>
@@ -3192,8 +3735,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I81" s="2"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>107</v>
       </c>
@@ -3215,8 +3760,10 @@
         <f t="shared" si="5"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I82" s="2"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>109</v>
       </c>
@@ -3238,8 +3785,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I83" s="2"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>106</v>
       </c>
@@ -3261,8 +3810,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I84" s="2"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>106</v>
       </c>
@@ -3284,8 +3835,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I85" s="2"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>109</v>
       </c>
@@ -3307,8 +3860,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I86" s="2"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>107</v>
       </c>
@@ -3330,8 +3885,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I87" s="2"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>107</v>
       </c>
@@ -3353,8 +3910,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I88" s="2"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>107</v>
       </c>
@@ -3376,8 +3935,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I89" s="2"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>109</v>
       </c>
@@ -3399,8 +3960,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I90" s="2"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>102</v>
       </c>
@@ -3422,8 +3985,10 @@
         <f t="shared" si="5"/>
         <v>0.92452830188679247</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I91" s="2"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>108</v>
       </c>
@@ -3445,8 +4010,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I92" s="2"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>104</v>
       </c>
@@ -3468,8 +4035,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I93" s="2"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>106</v>
       </c>
@@ -3491,8 +4060,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I94" s="2"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>100</v>
       </c>
@@ -3514,8 +4085,10 @@
         <f t="shared" si="5"/>
         <v>0.83018867924528306</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I95" s="2"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>109</v>
       </c>
@@ -3537,8 +4110,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I96" s="2"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>106</v>
       </c>
@@ -3560,8 +4135,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I97" s="2"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>106</v>
       </c>
@@ -3583,8 +4160,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I98" s="2"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>109</v>
       </c>
@@ -3606,8 +4185,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I99" s="2"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>109</v>
       </c>
@@ -3629,8 +4210,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I100" s="2"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>107</v>
       </c>
@@ -3652,8 +4235,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I101" s="2"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>109</v>
       </c>
@@ -3675,8 +4260,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I102" s="2"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>104</v>
       </c>
@@ -3698,8 +4285,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I103" s="2"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3721,8 +4310,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I104" s="2"/>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>108</v>
       </c>
@@ -3744,8 +4335,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I105" s="2"/>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>109</v>
       </c>
@@ -3767,8 +4360,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I106" s="2"/>
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>109</v>
       </c>
@@ -3790,8 +4385,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I107" s="2"/>
+      <c r="J107" s="3"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>109</v>
       </c>
@@ -3813,8 +4410,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I108" s="2"/>
+      <c r="J108" s="3"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3836,8 +4435,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I109" s="2"/>
+      <c r="J109" s="3"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3859,8 +4460,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I110" s="2"/>
+      <c r="J110" s="3"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>104</v>
       </c>
@@ -3882,8 +4485,10 @@
         <f t="shared" si="5"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I111" s="2"/>
+      <c r="J111" s="3"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>104</v>
       </c>
@@ -3905,8 +4510,10 @@
         <f t="shared" si="5"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I112" s="2"/>
+      <c r="J112" s="3"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>105</v>
       </c>
@@ -3928,8 +4535,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I113" s="2"/>
+      <c r="J113" s="3"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>103</v>
       </c>
@@ -3951,8 +4560,10 @@
         <f t="shared" si="5"/>
         <v>0.90566037735849059</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I114" s="2"/>
+      <c r="J114" s="3"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>109</v>
       </c>
@@ -3974,8 +4585,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I115" s="2"/>
+      <c r="J115" s="3"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>102</v>
       </c>
@@ -3997,8 +4610,10 @@
         <f t="shared" si="5"/>
         <v>0.90566037735849059</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I116" s="2"/>
+      <c r="J116" s="3"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>104</v>
       </c>
@@ -4020,8 +4635,10 @@
         <f t="shared" si="5"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I117" s="2"/>
+      <c r="J117" s="3"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>109</v>
       </c>
@@ -4043,8 +4660,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I118" s="2"/>
+      <c r="J118" s="3"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>105</v>
       </c>
@@ -4066,8 +4685,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I119" s="2"/>
+      <c r="J119" s="3"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>104</v>
       </c>
@@ -4089,8 +4710,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I120" s="2"/>
+      <c r="J120" s="3"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>102</v>
       </c>
@@ -4112,8 +4735,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I121" s="2"/>
+      <c r="J121" s="3"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>107</v>
       </c>
@@ -4135,8 +4760,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I122" s="2"/>
+      <c r="J122" s="3"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>100</v>
       </c>
@@ -4158,8 +4785,10 @@
         <f t="shared" si="5"/>
         <v>0.90566037735849059</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I123" s="2"/>
+      <c r="J123" s="3"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>109</v>
       </c>
@@ -4181,8 +4810,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I124" s="2"/>
+      <c r="J124" s="3"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>109</v>
       </c>
@@ -4204,8 +4835,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I125" s="2"/>
+      <c r="J125" s="3"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>109</v>
       </c>
@@ -4227,8 +4860,10 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I126" s="2"/>
+      <c r="J126" s="3"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>101</v>
       </c>
@@ -4250,8 +4885,10 @@
         <f t="shared" si="5"/>
         <v>0.8867924528301887</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I127" s="2"/>
+      <c r="J127" s="3"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>97</v>
       </c>
@@ -4273,8 +4910,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I128" s="2"/>
+      <c r="J128" s="3"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>102</v>
       </c>
@@ -4296,8 +4935,10 @@
         <f t="shared" si="5"/>
         <v>0.86792452830188682</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I129" s="2"/>
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>103</v>
       </c>
@@ -4319,8 +4960,10 @@
         <f t="shared" si="5"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I130" s="2"/>
+      <c r="J130" s="3"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>106</v>
       </c>
@@ -4342,8 +4985,10 @@
         <f t="shared" ref="F131:F194" si="8">C131/53</f>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I131" s="2"/>
+      <c r="J131" s="3"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>103</v>
       </c>
@@ -4365,8 +5010,10 @@
         <f t="shared" si="8"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I132" s="2"/>
+      <c r="J132" s="3"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>107</v>
       </c>
@@ -4388,8 +5035,10 @@
         <f t="shared" si="8"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I133" s="2"/>
+      <c r="J133" s="3"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>101</v>
       </c>
@@ -4411,8 +5060,10 @@
         <f t="shared" si="8"/>
         <v>0.8867924528301887</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I134" s="2"/>
+      <c r="J134" s="3"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>106</v>
       </c>
@@ -4434,8 +5085,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I135" s="2"/>
+      <c r="J135" s="3"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>104</v>
       </c>
@@ -4457,8 +5110,10 @@
         <f t="shared" si="8"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I136" s="2"/>
+      <c r="J136" s="3"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>99</v>
       </c>
@@ -4480,8 +5135,10 @@
         <f t="shared" si="8"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I137" s="2"/>
+      <c r="J137" s="3"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>104</v>
       </c>
@@ -4503,8 +5160,10 @@
         <f t="shared" si="8"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I138" s="2"/>
+      <c r="J138" s="3"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>108</v>
       </c>
@@ -4526,8 +5185,10 @@
         <f t="shared" si="8"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I139" s="2"/>
+      <c r="J139" s="3"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>105</v>
       </c>
@@ -4549,8 +5210,10 @@
         <f t="shared" si="8"/>
         <v>0.92452830188679247</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I140" s="2"/>
+      <c r="J140" s="3"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>101</v>
       </c>
@@ -4572,8 +5235,10 @@
         <f t="shared" si="8"/>
         <v>0.98113207547169812</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I141" s="2"/>
+      <c r="J141" s="3"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>106</v>
       </c>
@@ -4595,8 +5260,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I142" s="2"/>
+      <c r="J142" s="3"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>102</v>
       </c>
@@ -4618,8 +5285,10 @@
         <f t="shared" si="8"/>
         <v>0.90566037735849059</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I143" s="2"/>
+      <c r="J143" s="3"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>100</v>
       </c>
@@ -4641,8 +5310,10 @@
         <f t="shared" si="8"/>
         <v>0.8867924528301887</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I144" s="2"/>
+      <c r="J144" s="3"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>106</v>
       </c>
@@ -4664,8 +5335,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I145" s="2"/>
+      <c r="J145" s="3"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>103</v>
       </c>
@@ -4687,8 +5360,10 @@
         <f t="shared" si="8"/>
         <v>0.92452830188679247</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I146" s="2"/>
+      <c r="J146" s="3"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>106</v>
       </c>
@@ -4710,8 +5385,10 @@
         <f t="shared" si="8"/>
         <v>0.94339622641509435</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I147" s="2"/>
+      <c r="J147" s="3"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>107</v>
       </c>
@@ -4733,8 +5410,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I148" s="2"/>
+      <c r="J148" s="3"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>109</v>
       </c>
@@ -4756,8 +5435,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I149" s="2"/>
+      <c r="J149" s="3"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>104</v>
       </c>
@@ -4779,8 +5460,10 @@
         <f t="shared" si="8"/>
         <v>0.96226415094339623</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I150" s="2"/>
+      <c r="J150" s="3"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>108</v>
       </c>
@@ -4802,8 +5485,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I151" s="2"/>
+      <c r="J151" s="3"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>105</v>
       </c>
@@ -4826,7 +5511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>108</v>
       </c>
@@ -4849,7 +5534,7 @@
         <v>0.98113207547169812</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>106</v>
       </c>
@@ -4872,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>104</v>
       </c>
@@ -4895,7 +5580,7 @@
         <v>0.96226415094339623</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>104</v>
       </c>
@@ -4918,7 +5603,7 @@
         <v>0.96226415094339623</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>103</v>
       </c>
@@ -4941,7 +5626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>98</v>
       </c>
@@ -4964,7 +5649,7 @@
         <v>0.83018867924528306</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>102</v>
       </c>
@@ -4987,7 +5672,7 @@
         <v>0.94339622641509435</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>102</v>
       </c>

</xml_diff>